<commit_message>
changes values in metrics ASIO_Izertis_FAIR_evaluation_v3
</commit_message>
<xml_diff>
--- a/entregables_hito_1/06-Métricas_FAIR/ASIO_Izertis_FAIR_evaluation_v3.xlsx
+++ b/entregables_hito_1/06-Métricas_FAIR/ASIO_Izertis_FAIR_evaluation_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\druiz\repositorios\UM\fair-metrics-evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{39DCCAB4-6CE4-4FA8-987D-4670896BF66F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88181BF9-D378-4FAD-AE9D-78DDB0C2693A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LEVELS" sheetId="5" r:id="rId1"/>
@@ -1167,7 +1167,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1421,6 +1421,41 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1482,40 +1517,8 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7502,19 +7505,19 @@
   <sheetData>
     <row r="2" spans="2:9" ht="13.2"/>
     <row r="3" spans="2:9" ht="30" customHeight="1">
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="105" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
+      <c r="C3" s="105"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="105"/>
+      <c r="F3" s="105"/>
+      <c r="G3" s="105"/>
+      <c r="H3" s="105"/>
+      <c r="I3" s="105"/>
     </row>
     <row r="5" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B5" s="92" t="s">
+      <c r="B5" s="104" t="s">
         <v>91</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -7525,7 +7528,7 @@
       </c>
     </row>
     <row r="6" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B6" s="92"/>
+      <c r="B6" s="104"/>
       <c r="C6" s="41" t="s">
         <v>76</v>
       </c>
@@ -7534,7 +7537,7 @@
       </c>
     </row>
     <row r="7" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B7" s="92"/>
+      <c r="B7" s="104"/>
       <c r="C7" s="42" t="s">
         <v>79</v>
       </c>
@@ -7543,7 +7546,7 @@
       </c>
     </row>
     <row r="8" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B8" s="92"/>
+      <c r="B8" s="104"/>
       <c r="C8" s="43" t="s">
         <v>82</v>
       </c>
@@ -7552,7 +7555,7 @@
       </c>
     </row>
     <row r="9" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B9" s="92"/>
+      <c r="B9" s="104"/>
       <c r="C9" s="44" t="s">
         <v>85</v>
       </c>
@@ -7561,7 +7564,7 @@
       </c>
     </row>
     <row r="10" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B10" s="92"/>
+      <c r="B10" s="104"/>
       <c r="C10" s="45" t="s">
         <v>87</v>
       </c>
@@ -7570,63 +7573,63 @@
       </c>
     </row>
     <row r="31" spans="2:9" ht="30" customHeight="1">
-      <c r="B31" s="93" t="s">
+      <c r="B31" s="105" t="s">
         <v>99</v>
       </c>
-      <c r="C31" s="93"/>
-      <c r="D31" s="93"/>
-      <c r="E31" s="93"/>
-      <c r="F31" s="93"/>
-      <c r="G31" s="93"/>
-      <c r="H31" s="93"/>
-      <c r="I31" s="93"/>
+      <c r="C31" s="105"/>
+      <c r="D31" s="105"/>
+      <c r="E31" s="105"/>
+      <c r="F31" s="105"/>
+      <c r="G31" s="105"/>
+      <c r="H31" s="105"/>
+      <c r="I31" s="105"/>
     </row>
     <row r="33" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B33" s="92" t="s">
+      <c r="B33" s="104" t="s">
         <v>93</v>
       </c>
-      <c r="C33" s="94" t="s">
+      <c r="C33" s="106" t="s">
         <v>75</v>
       </c>
-      <c r="D33" s="94"/>
-      <c r="E33" s="94"/>
-      <c r="F33" s="94"/>
+      <c r="D33" s="106"/>
+      <c r="E33" s="106"/>
+      <c r="F33" s="106"/>
     </row>
     <row r="34" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B34" s="92"/>
-      <c r="C34" s="95" t="s">
+      <c r="B34" s="104"/>
+      <c r="C34" s="107" t="s">
         <v>62</v>
       </c>
-      <c r="D34" s="95"/>
-      <c r="E34" s="95"/>
-      <c r="F34" s="95"/>
+      <c r="D34" s="107"/>
+      <c r="E34" s="107"/>
+      <c r="F34" s="107"/>
     </row>
     <row r="35" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B35" s="92"/>
-      <c r="C35" s="96" t="s">
+      <c r="B35" s="104"/>
+      <c r="C35" s="108" t="s">
         <v>60</v>
       </c>
-      <c r="D35" s="96"/>
-      <c r="E35" s="96"/>
-      <c r="F35" s="96"/>
+      <c r="D35" s="108"/>
+      <c r="E35" s="108"/>
+      <c r="F35" s="108"/>
     </row>
     <row r="36" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B36" s="92"/>
-      <c r="C36" s="97" t="s">
+      <c r="B36" s="104"/>
+      <c r="C36" s="109" t="s">
         <v>61</v>
       </c>
-      <c r="D36" s="97"/>
-      <c r="E36" s="97"/>
-      <c r="F36" s="97"/>
+      <c r="D36" s="109"/>
+      <c r="E36" s="109"/>
+      <c r="F36" s="109"/>
     </row>
     <row r="37" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B37" s="92"/>
-      <c r="C37" s="98" t="s">
+      <c r="B37" s="104"/>
+      <c r="C37" s="110" t="s">
         <v>64</v>
       </c>
-      <c r="D37" s="98"/>
-      <c r="E37" s="98"/>
-      <c r="F37" s="98"/>
+      <c r="D37" s="110"/>
+      <c r="E37" s="110"/>
+      <c r="F37" s="110"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-1" hashValue="6rQiKCLsP3fGx3S8B0laN7bDPnU=" saltValue="flfJfApD/MGgsX1wXY6YWQ==" spinCount="100000" sheet="1" selectLockedCells="1" selectUnlockedCells="1"/>
@@ -7724,7 +7727,7 @@
       <c r="A2" s="51">
         <v>1</v>
       </c>
-      <c r="B2" s="102" t="str">
+      <c r="B2" s="114" t="str">
         <f>LEFT(D2)</f>
         <v>F</v>
       </c>
@@ -7785,7 +7788,7 @@
       <c r="A3" s="51">
         <v>2</v>
       </c>
-      <c r="B3" s="103"/>
+      <c r="B3" s="115"/>
       <c r="C3" s="52" t="str">
         <f t="shared" si="0"/>
         <v>F</v>
@@ -7843,7 +7846,7 @@
       <c r="A4" s="51">
         <v>3</v>
       </c>
-      <c r="B4" s="103"/>
+      <c r="B4" s="115"/>
       <c r="C4" s="52" t="str">
         <f t="shared" si="0"/>
         <v>F</v>
@@ -7901,7 +7904,7 @@
       <c r="A5" s="51">
         <v>4</v>
       </c>
-      <c r="B5" s="103"/>
+      <c r="B5" s="115"/>
       <c r="C5" s="52" t="str">
         <f t="shared" si="0"/>
         <v>F</v>
@@ -7959,7 +7962,7 @@
       <c r="A6" s="51">
         <v>5</v>
       </c>
-      <c r="B6" s="103"/>
+      <c r="B6" s="115"/>
       <c r="C6" s="52" t="str">
         <f t="shared" si="0"/>
         <v>F</v>
@@ -8017,7 +8020,7 @@
       <c r="A7" s="51">
         <v>6</v>
       </c>
-      <c r="B7" s="103"/>
+      <c r="B7" s="115"/>
       <c r="C7" s="52" t="str">
         <f t="shared" si="0"/>
         <v>F</v>
@@ -8075,7 +8078,7 @@
       <c r="A8" s="51">
         <v>7</v>
       </c>
-      <c r="B8" s="103"/>
+      <c r="B8" s="115"/>
       <c r="C8" s="52" t="str">
         <f t="shared" si="0"/>
         <v>F</v>
@@ -8133,7 +8136,7 @@
       <c r="A9" s="51">
         <v>8</v>
       </c>
-      <c r="B9" s="104" t="str">
+      <c r="B9" s="116" t="str">
         <f>LEFT(D9)</f>
         <v>A</v>
       </c>
@@ -8194,7 +8197,7 @@
       <c r="A10" s="51">
         <v>9</v>
       </c>
-      <c r="B10" s="105"/>
+      <c r="B10" s="117"/>
       <c r="C10" s="56" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
@@ -8252,7 +8255,7 @@
       <c r="A11" s="51">
         <v>10</v>
       </c>
-      <c r="B11" s="105"/>
+      <c r="B11" s="117"/>
       <c r="C11" s="56" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
@@ -8310,7 +8313,7 @@
       <c r="A12" s="51">
         <v>11</v>
       </c>
-      <c r="B12" s="105"/>
+      <c r="B12" s="117"/>
       <c r="C12" s="56" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
@@ -8368,7 +8371,7 @@
       <c r="A13" s="51">
         <v>12</v>
       </c>
-      <c r="B13" s="105"/>
+      <c r="B13" s="117"/>
       <c r="C13" s="56" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
@@ -8426,7 +8429,7 @@
       <c r="A14" s="51">
         <v>13</v>
       </c>
-      <c r="B14" s="105"/>
+      <c r="B14" s="117"/>
       <c r="C14" s="56" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
@@ -8484,7 +8487,7 @@
       <c r="A15" s="51">
         <v>14</v>
       </c>
-      <c r="B15" s="105"/>
+      <c r="B15" s="117"/>
       <c r="C15" s="56" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
@@ -8542,7 +8545,7 @@
       <c r="A16" s="51">
         <v>15</v>
       </c>
-      <c r="B16" s="105"/>
+      <c r="B16" s="117"/>
       <c r="C16" s="56" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
@@ -8600,7 +8603,7 @@
       <c r="A17" s="51">
         <v>16</v>
       </c>
-      <c r="B17" s="105"/>
+      <c r="B17" s="117"/>
       <c r="C17" s="56" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
@@ -8658,7 +8661,7 @@
       <c r="A18" s="51">
         <v>17</v>
       </c>
-      <c r="B18" s="105"/>
+      <c r="B18" s="117"/>
       <c r="C18" s="56" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
@@ -8716,7 +8719,7 @@
       <c r="A19" s="51">
         <v>18</v>
       </c>
-      <c r="B19" s="105"/>
+      <c r="B19" s="117"/>
       <c r="C19" s="56" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
@@ -8774,7 +8777,7 @@
       <c r="A20" s="51">
         <v>19</v>
       </c>
-      <c r="B20" s="106"/>
+      <c r="B20" s="118"/>
       <c r="C20" s="56" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
@@ -8832,7 +8835,7 @@
       <c r="A21" s="51">
         <v>20</v>
       </c>
-      <c r="B21" s="107" t="str">
+      <c r="B21" s="119" t="str">
         <f>LEFT(D25)</f>
         <v>I</v>
       </c>
@@ -8893,7 +8896,7 @@
       <c r="A22" s="51">
         <v>21</v>
       </c>
-      <c r="B22" s="108"/>
+      <c r="B22" s="120"/>
       <c r="C22" s="56" t="str">
         <f t="shared" si="0"/>
         <v>I</v>
@@ -8951,7 +8954,7 @@
       <c r="A23" s="51">
         <v>22</v>
       </c>
-      <c r="B23" s="108"/>
+      <c r="B23" s="120"/>
       <c r="C23" s="56" t="str">
         <f t="shared" si="0"/>
         <v>I</v>
@@ -9009,7 +9012,7 @@
       <c r="A24" s="51">
         <v>23</v>
       </c>
-      <c r="B24" s="108"/>
+      <c r="B24" s="120"/>
       <c r="C24" s="56" t="str">
         <f t="shared" si="0"/>
         <v>I</v>
@@ -9067,7 +9070,7 @@
       <c r="A25" s="51">
         <v>24</v>
       </c>
-      <c r="B25" s="108"/>
+      <c r="B25" s="120"/>
       <c r="C25" s="58" t="str">
         <f t="shared" si="0"/>
         <v>I</v>
@@ -9125,7 +9128,7 @@
       <c r="A26" s="51">
         <v>25</v>
       </c>
-      <c r="B26" s="108"/>
+      <c r="B26" s="120"/>
       <c r="C26" s="58" t="str">
         <f t="shared" si="0"/>
         <v>I</v>
@@ -9183,7 +9186,7 @@
       <c r="A27" s="51">
         <v>26</v>
       </c>
-      <c r="B27" s="108"/>
+      <c r="B27" s="120"/>
       <c r="C27" s="58" t="str">
         <f t="shared" si="0"/>
         <v>I</v>
@@ -9241,7 +9244,7 @@
       <c r="A28" s="51">
         <v>27</v>
       </c>
-      <c r="B28" s="108"/>
+      <c r="B28" s="120"/>
       <c r="C28" s="58" t="str">
         <f t="shared" si="0"/>
         <v>I</v>
@@ -9299,7 +9302,7 @@
       <c r="A29" s="51">
         <v>28</v>
       </c>
-      <c r="B29" s="108"/>
+      <c r="B29" s="120"/>
       <c r="C29" s="58" t="str">
         <f t="shared" si="0"/>
         <v>I</v>
@@ -9357,7 +9360,7 @@
       <c r="A30" s="51">
         <v>29</v>
       </c>
-      <c r="B30" s="108"/>
+      <c r="B30" s="120"/>
       <c r="C30" s="58" t="str">
         <f t="shared" si="0"/>
         <v>I</v>
@@ -9415,7 +9418,7 @@
       <c r="A31" s="51">
         <v>30</v>
       </c>
-      <c r="B31" s="108"/>
+      <c r="B31" s="120"/>
       <c r="C31" s="58" t="str">
         <f t="shared" si="0"/>
         <v>I</v>
@@ -9473,7 +9476,7 @@
       <c r="A32" s="51">
         <v>31</v>
       </c>
-      <c r="B32" s="109"/>
+      <c r="B32" s="121"/>
       <c r="C32" s="58" t="str">
         <f t="shared" si="0"/>
         <v>I</v>
@@ -9531,7 +9534,7 @@
       <c r="A33" s="51">
         <v>32</v>
       </c>
-      <c r="B33" s="99" t="str">
+      <c r="B33" s="111" t="str">
         <f>LEFT(D41)</f>
         <v>R</v>
       </c>
@@ -9592,7 +9595,7 @@
       <c r="A34" s="51">
         <v>33</v>
       </c>
-      <c r="B34" s="100"/>
+      <c r="B34" s="112"/>
       <c r="C34" s="58" t="str">
         <f t="shared" si="0"/>
         <v>R</v>
@@ -9650,7 +9653,7 @@
       <c r="A35" s="51">
         <v>34</v>
       </c>
-      <c r="B35" s="100"/>
+      <c r="B35" s="112"/>
       <c r="C35" s="58" t="str">
         <f t="shared" si="0"/>
         <v>R</v>
@@ -9708,7 +9711,7 @@
       <c r="A36" s="51">
         <v>35</v>
       </c>
-      <c r="B36" s="100"/>
+      <c r="B36" s="112"/>
       <c r="C36" s="58" t="str">
         <f t="shared" si="0"/>
         <v>R</v>
@@ -9766,7 +9769,7 @@
       <c r="A37" s="51">
         <v>36</v>
       </c>
-      <c r="B37" s="100"/>
+      <c r="B37" s="112"/>
       <c r="C37" s="58" t="str">
         <f t="shared" si="0"/>
         <v>R</v>
@@ -9824,7 +9827,7 @@
       <c r="A38" s="51">
         <v>37</v>
       </c>
-      <c r="B38" s="100"/>
+      <c r="B38" s="112"/>
       <c r="C38" s="58" t="str">
         <f t="shared" si="0"/>
         <v>R</v>
@@ -9882,7 +9885,7 @@
       <c r="A39" s="51">
         <v>38</v>
       </c>
-      <c r="B39" s="100"/>
+      <c r="B39" s="112"/>
       <c r="C39" s="58" t="str">
         <f t="shared" si="0"/>
         <v>R</v>
@@ -9940,7 +9943,7 @@
       <c r="A40" s="51">
         <v>39</v>
       </c>
-      <c r="B40" s="100"/>
+      <c r="B40" s="112"/>
       <c r="C40" s="58" t="str">
         <f t="shared" si="0"/>
         <v>R</v>
@@ -9998,7 +10001,7 @@
       <c r="A41" s="51">
         <v>40</v>
       </c>
-      <c r="B41" s="100"/>
+      <c r="B41" s="112"/>
       <c r="C41" s="59" t="str">
         <f t="shared" si="0"/>
         <v>R</v>
@@ -10056,7 +10059,7 @@
       <c r="A42" s="51">
         <v>41</v>
       </c>
-      <c r="B42" s="101"/>
+      <c r="B42" s="113"/>
       <c r="C42" s="59" t="str">
         <f t="shared" si="0"/>
         <v>R</v>
@@ -36708,7 +36711,7 @@
   </sheetPr>
   <dimension ref="A1:U44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="H10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
@@ -36770,7 +36773,7 @@
       <c r="A2" s="51">
         <v>1</v>
       </c>
-      <c r="B2" s="110" t="str">
+      <c r="B2" s="122" t="str">
         <f>LEFT(D2)</f>
         <v>F</v>
       </c>
@@ -36781,7 +36784,7 @@
       <c r="D2" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="113" t="s">
+      <c r="E2" s="92" t="s">
         <v>101</v>
       </c>
       <c r="F2" s="53" t="s">
@@ -36812,7 +36815,7 @@
       <c r="A3" s="51">
         <v>2</v>
       </c>
-      <c r="B3" s="111"/>
+      <c r="B3" s="123"/>
       <c r="C3" s="52" t="str">
         <f t="shared" si="0"/>
         <v>F</v>
@@ -36820,7 +36823,7 @@
       <c r="D3" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="114" t="s">
+      <c r="E3" s="93" t="s">
         <v>102</v>
       </c>
       <c r="F3" s="53" t="s">
@@ -36851,7 +36854,7 @@
       <c r="A4" s="51">
         <v>3</v>
       </c>
-      <c r="B4" s="111"/>
+      <c r="B4" s="123"/>
       <c r="C4" s="52" t="str">
         <f t="shared" si="0"/>
         <v>F</v>
@@ -36859,7 +36862,7 @@
       <c r="D4" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="114" t="s">
+      <c r="E4" s="93" t="s">
         <v>103</v>
       </c>
       <c r="F4" s="53" t="s">
@@ -36890,7 +36893,7 @@
       <c r="A5" s="51">
         <v>4</v>
       </c>
-      <c r="B5" s="111"/>
+      <c r="B5" s="123"/>
       <c r="C5" s="52" t="str">
         <f t="shared" si="0"/>
         <v>F</v>
@@ -36898,7 +36901,7 @@
       <c r="D5" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="114" t="s">
+      <c r="E5" s="93" t="s">
         <v>105</v>
       </c>
       <c r="F5" s="53" t="s">
@@ -36929,7 +36932,7 @@
       <c r="A6" s="51">
         <v>5</v>
       </c>
-      <c r="B6" s="111"/>
+      <c r="B6" s="123"/>
       <c r="C6" s="52" t="str">
         <f t="shared" si="0"/>
         <v>F</v>
@@ -36937,7 +36940,7 @@
       <c r="D6" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="114" t="s">
+      <c r="E6" s="93" t="s">
         <v>107</v>
       </c>
       <c r="F6" s="53" t="s">
@@ -36968,7 +36971,7 @@
       <c r="A7" s="82">
         <v>6</v>
       </c>
-      <c r="B7" s="111"/>
+      <c r="B7" s="123"/>
       <c r="C7" s="52" t="str">
         <f t="shared" si="0"/>
         <v>F</v>
@@ -36976,7 +36979,7 @@
       <c r="D7" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="114" t="s">
+      <c r="E7" s="93" t="s">
         <v>109</v>
       </c>
       <c r="F7" s="53" t="s">
@@ -37007,38 +37010,38 @@
       <c r="A8" s="82">
         <v>7</v>
       </c>
-      <c r="B8" s="112"/>
+      <c r="B8" s="124"/>
       <c r="C8" s="52" t="str">
         <f t="shared" si="0"/>
         <v>F</v>
       </c>
-      <c r="D8" s="115" t="s">
+      <c r="D8" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="115" t="s">
+      <c r="E8" s="94" t="s">
         <v>110</v>
       </c>
-      <c r="F8" s="116" t="s">
+      <c r="F8" s="95" t="s">
         <v>111</v>
       </c>
-      <c r="G8" s="117" t="s">
+      <c r="G8" s="96" t="s">
         <v>59</v>
       </c>
-      <c r="H8" s="118" t="s">
+      <c r="H8" s="97" t="s">
         <v>64</v>
       </c>
-      <c r="I8" s="119">
+      <c r="I8" s="98">
         <f>IF($H8="","",IF($H8=DATA!$L$1,0,IF($H8=DATA!$L$2,1,IF($H8=DATA!$L$3,2,IF($H8=DATA!$L$4,3,4)))))</f>
         <v>4</v>
       </c>
-      <c r="J8" s="120">
+      <c r="J8" s="99">
         <f>IF(OR($H8=DATA!$L$1,$H8=DATA!$L$2,$H8=DATA!$L$3,$H8=DATA!$L$4,$H8=0),0,1)</f>
         <v>1</v>
       </c>
-      <c r="K8" s="116" t="s">
+      <c r="K8" s="95" t="s">
         <v>155</v>
       </c>
-      <c r="L8" s="121">
+      <c r="L8" s="100">
         <v>0</v>
       </c>
     </row>
@@ -37046,7 +37049,7 @@
       <c r="A9" s="70">
         <v>8</v>
       </c>
-      <c r="B9" s="104" t="str">
+      <c r="B9" s="116" t="str">
         <f>LEFT(D9)</f>
         <v>A</v>
       </c>
@@ -37057,7 +37060,7 @@
       <c r="D9" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="122" t="s">
+      <c r="E9" s="101" t="s">
         <v>112</v>
       </c>
       <c r="F9" s="77" t="s">
@@ -37088,38 +37091,38 @@
       <c r="A10" s="82">
         <v>9</v>
       </c>
-      <c r="B10" s="105"/>
+      <c r="B10" s="117"/>
       <c r="C10" s="56" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
       </c>
-      <c r="D10" s="115" t="s">
+      <c r="D10" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="115" t="s">
+      <c r="E10" s="94" t="s">
         <v>114</v>
       </c>
-      <c r="F10" s="116" t="s">
+      <c r="F10" s="95" t="s">
         <v>115</v>
       </c>
-      <c r="G10" s="117" t="s">
+      <c r="G10" s="96" t="s">
         <v>59</v>
       </c>
-      <c r="H10" s="118" t="s">
+      <c r="H10" s="97" t="s">
         <v>64</v>
       </c>
-      <c r="I10" s="119">
+      <c r="I10" s="98">
         <f>IF($H10="","",IF($H10=DATA!$L$1,0,IF($H10=DATA!$L$2,1,IF($H10=DATA!$L$3,2,IF($H10=DATA!$L$4,3,4)))))</f>
         <v>4</v>
       </c>
-      <c r="J10" s="120">
+      <c r="J10" s="99">
         <f>IF(OR($H10=DATA!$L$1,$H10=DATA!$L$2,$H10=DATA!$L$3,$H10=DATA!$L$4,$H10=0),0,1)</f>
         <v>1</v>
       </c>
-      <c r="K10" s="116" t="s">
+      <c r="K10" s="95" t="s">
         <v>158</v>
       </c>
-      <c r="L10" s="121">
+      <c r="L10" s="100">
         <v>0</v>
       </c>
     </row>
@@ -37127,38 +37130,38 @@
       <c r="A11" s="82">
         <v>10</v>
       </c>
-      <c r="B11" s="105"/>
+      <c r="B11" s="117"/>
       <c r="C11" s="56" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
       </c>
-      <c r="D11" s="115" t="s">
+      <c r="D11" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="115" t="s">
+      <c r="E11" s="94" t="s">
         <v>116</v>
       </c>
-      <c r="F11" s="116" t="s">
+      <c r="F11" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="117" t="s">
+      <c r="G11" s="96" t="s">
         <v>59</v>
       </c>
-      <c r="H11" s="118" t="s">
+      <c r="H11" s="97" t="s">
         <v>64</v>
       </c>
-      <c r="I11" s="119">
+      <c r="I11" s="98">
         <f>IF($H11="","",IF($H11=DATA!$L$1,0,IF($H11=DATA!$L$2,1,IF($H11=DATA!$L$3,2,IF($H11=DATA!$L$4,3,4)))))</f>
         <v>4</v>
       </c>
-      <c r="J11" s="120">
+      <c r="J11" s="99">
         <f>IF(OR($H11=DATA!$L$1,$H11=DATA!$L$2,$H11=DATA!$L$3,$H11=DATA!$L$4,$H11=0),0,1)</f>
         <v>1</v>
       </c>
-      <c r="K11" s="116" t="s">
+      <c r="K11" s="95" t="s">
         <v>159</v>
       </c>
-      <c r="L11" s="121">
+      <c r="L11" s="100">
         <v>0</v>
       </c>
     </row>
@@ -37166,7 +37169,7 @@
       <c r="A12" s="51">
         <v>11</v>
       </c>
-      <c r="B12" s="105"/>
+      <c r="B12" s="117"/>
       <c r="C12" s="56" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
@@ -37174,10 +37177,10 @@
       <c r="D12" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="114" t="s">
+      <c r="E12" s="93" t="s">
         <v>117</v>
       </c>
-      <c r="F12" s="123" t="s">
+      <c r="F12" s="102" t="s">
         <v>19</v>
       </c>
       <c r="G12" s="60" t="s">
@@ -37205,7 +37208,7 @@
       <c r="A13" s="51">
         <v>12</v>
       </c>
-      <c r="B13" s="105"/>
+      <c r="B13" s="117"/>
       <c r="C13" s="56" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
@@ -37213,7 +37216,7 @@
       <c r="D13" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="114" t="s">
+      <c r="E13" s="93" t="s">
         <v>118</v>
       </c>
       <c r="F13" s="53" t="s">
@@ -37244,7 +37247,7 @@
       <c r="A14" s="51">
         <v>13</v>
       </c>
-      <c r="B14" s="105"/>
+      <c r="B14" s="117"/>
       <c r="C14" s="56" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
@@ -37252,7 +37255,7 @@
       <c r="D14" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="114" t="s">
+      <c r="E14" s="93" t="s">
         <v>119</v>
       </c>
       <c r="F14" s="53" t="s">
@@ -37283,7 +37286,7 @@
       <c r="A15" s="51">
         <v>14</v>
       </c>
-      <c r="B15" s="105"/>
+      <c r="B15" s="117"/>
       <c r="C15" s="56" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
@@ -37291,7 +37294,7 @@
       <c r="D15" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="114" t="s">
+      <c r="E15" s="93" t="s">
         <v>120</v>
       </c>
       <c r="F15" s="53" t="s">
@@ -37322,7 +37325,7 @@
       <c r="A16" s="51">
         <v>15</v>
       </c>
-      <c r="B16" s="105"/>
+      <c r="B16" s="117"/>
       <c r="C16" s="56" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
@@ -37330,7 +37333,7 @@
       <c r="D16" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="114" t="s">
+      <c r="E16" s="93" t="s">
         <v>121</v>
       </c>
       <c r="F16" s="55" t="s">
@@ -37361,7 +37364,7 @@
       <c r="A17" s="51">
         <v>16</v>
       </c>
-      <c r="B17" s="105"/>
+      <c r="B17" s="117"/>
       <c r="C17" s="56" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
@@ -37369,10 +37372,10 @@
       <c r="D17" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="114" t="s">
+      <c r="E17" s="93" t="s">
         <v>122</v>
       </c>
-      <c r="F17" s="123" t="s">
+      <c r="F17" s="102" t="s">
         <v>24</v>
       </c>
       <c r="G17" s="60" t="s">
@@ -37400,7 +37403,7 @@
       <c r="A18" s="51">
         <v>17</v>
       </c>
-      <c r="B18" s="105"/>
+      <c r="B18" s="117"/>
       <c r="C18" s="56" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
@@ -37408,7 +37411,7 @@
       <c r="D18" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="114" t="s">
+      <c r="E18" s="93" t="s">
         <v>123</v>
       </c>
       <c r="F18" s="55" t="s">
@@ -37439,7 +37442,7 @@
       <c r="A19" s="51">
         <v>18</v>
       </c>
-      <c r="B19" s="105"/>
+      <c r="B19" s="117"/>
       <c r="C19" s="56" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
@@ -37447,7 +37450,7 @@
       <c r="D19" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="114" t="s">
+      <c r="E19" s="93" t="s">
         <v>124</v>
       </c>
       <c r="F19" s="57" t="s">
@@ -37478,7 +37481,7 @@
       <c r="A20" s="82">
         <v>19</v>
       </c>
-      <c r="B20" s="106"/>
+      <c r="B20" s="118"/>
       <c r="C20" s="56" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
@@ -37486,7 +37489,7 @@
       <c r="D20" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="114" t="s">
+      <c r="E20" s="93" t="s">
         <v>126</v>
       </c>
       <c r="F20" s="53" t="s">
@@ -37517,7 +37520,7 @@
       <c r="A21" s="51">
         <v>20</v>
       </c>
-      <c r="B21" s="107" t="str">
+      <c r="B21" s="119" t="str">
         <f>LEFT(D25)</f>
         <v>I</v>
       </c>
@@ -37528,7 +37531,7 @@
       <c r="D21" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="114" t="s">
+      <c r="E21" s="93" t="s">
         <v>127</v>
       </c>
       <c r="F21" s="55" t="s">
@@ -37559,7 +37562,7 @@
       <c r="A22" s="51">
         <v>21</v>
       </c>
-      <c r="B22" s="108"/>
+      <c r="B22" s="120"/>
       <c r="C22" s="56" t="str">
         <f t="shared" si="0"/>
         <v>I</v>
@@ -37567,7 +37570,7 @@
       <c r="D22" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="114" t="s">
+      <c r="E22" s="93" t="s">
         <v>128</v>
       </c>
       <c r="F22" s="55" t="s">
@@ -37598,7 +37601,7 @@
       <c r="A23" s="51">
         <v>22</v>
       </c>
-      <c r="B23" s="108"/>
+      <c r="B23" s="120"/>
       <c r="C23" s="56" t="str">
         <f t="shared" si="0"/>
         <v>I</v>
@@ -37606,7 +37609,7 @@
       <c r="D23" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="114" t="s">
+      <c r="E23" s="93" t="s">
         <v>129</v>
       </c>
       <c r="F23" s="55" t="s">
@@ -37637,7 +37640,7 @@
       <c r="A24" s="51">
         <v>23</v>
       </c>
-      <c r="B24" s="108"/>
+      <c r="B24" s="120"/>
       <c r="C24" s="56" t="str">
         <f t="shared" si="0"/>
         <v>I</v>
@@ -37645,7 +37648,7 @@
       <c r="D24" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="114" t="s">
+      <c r="E24" s="93" t="s">
         <v>130</v>
       </c>
       <c r="F24" s="55" t="s">
@@ -37676,7 +37679,7 @@
       <c r="A25" s="51">
         <v>24</v>
       </c>
-      <c r="B25" s="108"/>
+      <c r="B25" s="120"/>
       <c r="C25" s="58" t="str">
         <f t="shared" si="0"/>
         <v>I</v>
@@ -37684,7 +37687,7 @@
       <c r="D25" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="E25" s="115" t="s">
+      <c r="E25" s="94" t="s">
         <v>131</v>
       </c>
       <c r="F25" s="55" t="s">
@@ -37715,7 +37718,7 @@
       <c r="A26" s="51">
         <v>25</v>
       </c>
-      <c r="B26" s="108"/>
+      <c r="B26" s="120"/>
       <c r="C26" s="58" t="str">
         <f t="shared" si="0"/>
         <v>I</v>
@@ -37723,7 +37726,7 @@
       <c r="D26" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="E26" s="115" t="s">
+      <c r="E26" s="94" t="s">
         <v>132</v>
       </c>
       <c r="F26" s="57" t="s">
@@ -37754,7 +37757,7 @@
       <c r="A27" s="82">
         <v>26</v>
       </c>
-      <c r="B27" s="108"/>
+      <c r="B27" s="120"/>
       <c r="C27" s="58" t="str">
         <f t="shared" si="0"/>
         <v>I</v>
@@ -37762,7 +37765,7 @@
       <c r="D27" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="E27" s="114" t="s">
+      <c r="E27" s="93" t="s">
         <v>133</v>
       </c>
       <c r="F27" s="55" t="s">
@@ -37793,7 +37796,7 @@
       <c r="A28" s="82">
         <v>27</v>
       </c>
-      <c r="B28" s="108"/>
+      <c r="B28" s="120"/>
       <c r="C28" s="58" t="str">
         <f t="shared" si="0"/>
         <v>I</v>
@@ -37801,7 +37804,7 @@
       <c r="D28" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="E28" s="114" t="s">
+      <c r="E28" s="93" t="s">
         <v>134</v>
       </c>
       <c r="F28" s="57" t="s">
@@ -37832,7 +37835,7 @@
       <c r="A29" s="70">
         <v>28</v>
       </c>
-      <c r="B29" s="108"/>
+      <c r="B29" s="120"/>
       <c r="C29" s="79" t="str">
         <f t="shared" si="0"/>
         <v>I</v>
@@ -37840,7 +37843,7 @@
       <c r="D29" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="E29" s="124" t="s">
+      <c r="E29" s="103" t="s">
         <v>135</v>
       </c>
       <c r="F29" s="80" t="s">
@@ -37871,7 +37874,7 @@
       <c r="A30" s="70">
         <v>29</v>
       </c>
-      <c r="B30" s="108"/>
+      <c r="B30" s="120"/>
       <c r="C30" s="79" t="str">
         <f t="shared" si="0"/>
         <v>I</v>
@@ -37879,7 +37882,7 @@
       <c r="D30" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="E30" s="124" t="s">
+      <c r="E30" s="103" t="s">
         <v>136</v>
       </c>
       <c r="F30" s="80" t="s">
@@ -37910,7 +37913,7 @@
       <c r="A31" s="70">
         <v>30</v>
       </c>
-      <c r="B31" s="108"/>
+      <c r="B31" s="120"/>
       <c r="C31" s="79" t="str">
         <f t="shared" si="0"/>
         <v>I</v>
@@ -37918,7 +37921,7 @@
       <c r="D31" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="E31" s="124" t="s">
+      <c r="E31" s="103" t="s">
         <v>138</v>
       </c>
       <c r="F31" s="77" t="s">
@@ -37949,7 +37952,7 @@
       <c r="A32" s="70">
         <v>31</v>
       </c>
-      <c r="B32" s="109"/>
+      <c r="B32" s="121"/>
       <c r="C32" s="79" t="str">
         <f t="shared" si="0"/>
         <v>I</v>
@@ -37957,7 +37960,7 @@
       <c r="D32" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="E32" s="124" t="s">
+      <c r="E32" s="103" t="s">
         <v>140</v>
       </c>
       <c r="F32" s="80" t="s">
@@ -37988,7 +37991,7 @@
       <c r="A33" s="70">
         <v>32</v>
       </c>
-      <c r="B33" s="99" t="str">
+      <c r="B33" s="111" t="str">
         <f>LEFT(D41)</f>
         <v>R</v>
       </c>
@@ -37999,7 +38002,7 @@
       <c r="D33" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="E33" s="122" t="s">
+      <c r="E33" s="101" t="s">
         <v>142</v>
       </c>
       <c r="F33" s="71" t="s">
@@ -38030,7 +38033,7 @@
       <c r="A34" s="82">
         <v>33</v>
       </c>
-      <c r="B34" s="100"/>
+      <c r="B34" s="112"/>
       <c r="C34" s="58" t="str">
         <f t="shared" si="0"/>
         <v>R</v>
@@ -38038,7 +38041,7 @@
       <c r="D34" s="82" t="s">
         <v>43</v>
       </c>
-      <c r="E34" s="115" t="s">
+      <c r="E34" s="94" t="s">
         <v>144</v>
       </c>
       <c r="F34" s="53" t="s">
@@ -38069,7 +38072,7 @@
       <c r="A35" s="82">
         <v>34</v>
       </c>
-      <c r="B35" s="100"/>
+      <c r="B35" s="112"/>
       <c r="C35" s="58" t="str">
         <f t="shared" si="0"/>
         <v>R</v>
@@ -38077,7 +38080,7 @@
       <c r="D35" s="82" t="s">
         <v>43</v>
       </c>
-      <c r="E35" s="115" t="s">
+      <c r="E35" s="94" t="s">
         <v>145</v>
       </c>
       <c r="F35" s="55" t="s">
@@ -38108,7 +38111,7 @@
       <c r="A36" s="82">
         <v>35</v>
       </c>
-      <c r="B36" s="100"/>
+      <c r="B36" s="112"/>
       <c r="C36" s="58" t="str">
         <f t="shared" si="0"/>
         <v>R</v>
@@ -38116,7 +38119,7 @@
       <c r="D36" s="82" t="s">
         <v>43</v>
       </c>
-      <c r="E36" s="115" t="s">
+      <c r="E36" s="94" t="s">
         <v>146</v>
       </c>
       <c r="F36" s="55" t="s">
@@ -38147,7 +38150,7 @@
       <c r="A37" s="82">
         <v>36</v>
       </c>
-      <c r="B37" s="100"/>
+      <c r="B37" s="112"/>
       <c r="C37" s="58" t="str">
         <f t="shared" si="0"/>
         <v>R</v>
@@ -38155,7 +38158,7 @@
       <c r="D37" s="82" t="s">
         <v>47</v>
       </c>
-      <c r="E37" s="114" t="s">
+      <c r="E37" s="93" t="s">
         <v>147</v>
       </c>
       <c r="F37" s="55" t="s">
@@ -38186,7 +38189,7 @@
       <c r="A38" s="82">
         <v>37</v>
       </c>
-      <c r="B38" s="100"/>
+      <c r="B38" s="112"/>
       <c r="C38" s="58" t="str">
         <f t="shared" si="0"/>
         <v>R</v>
@@ -38194,7 +38197,7 @@
       <c r="D38" s="82" t="s">
         <v>47</v>
       </c>
-      <c r="E38" s="114" t="s">
+      <c r="E38" s="93" t="s">
         <v>148</v>
       </c>
       <c r="F38" s="57" t="s">
@@ -38225,7 +38228,7 @@
       <c r="A39" s="51">
         <v>38</v>
       </c>
-      <c r="B39" s="100"/>
+      <c r="B39" s="112"/>
       <c r="C39" s="58" t="str">
         <f t="shared" si="0"/>
         <v>R</v>
@@ -38233,7 +38236,7 @@
       <c r="D39" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="E39" s="114" t="s">
+      <c r="E39" s="93" t="s">
         <v>150</v>
       </c>
       <c r="F39" s="53" t="s">
@@ -38264,7 +38267,7 @@
       <c r="A40" s="51">
         <v>39</v>
       </c>
-      <c r="B40" s="100"/>
+      <c r="B40" s="112"/>
       <c r="C40" s="58" t="str">
         <f t="shared" si="0"/>
         <v>R</v>
@@ -38272,7 +38275,7 @@
       <c r="D40" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="E40" s="114" t="s">
+      <c r="E40" s="93" t="s">
         <v>151</v>
       </c>
       <c r="F40" s="53" t="s">
@@ -38303,7 +38306,7 @@
       <c r="A41" s="51">
         <v>40</v>
       </c>
-      <c r="B41" s="100"/>
+      <c r="B41" s="112"/>
       <c r="C41" s="59" t="str">
         <f t="shared" si="0"/>
         <v>R</v>
@@ -38311,7 +38314,7 @@
       <c r="D41" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="E41" s="114" t="s">
+      <c r="E41" s="93" t="s">
         <v>152</v>
       </c>
       <c r="F41" s="53" t="s">
@@ -38342,7 +38345,7 @@
       <c r="A42" s="51">
         <v>41</v>
       </c>
-      <c r="B42" s="101"/>
+      <c r="B42" s="113"/>
       <c r="C42" s="59" t="str">
         <f t="shared" si="0"/>
         <v>R</v>
@@ -38350,7 +38353,7 @@
       <c r="D42" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="E42" s="114" t="s">
+      <c r="E42" s="93" t="s">
         <v>153</v>
       </c>
       <c r="F42" s="55" t="s">
@@ -38429,8 +38432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E72AF82D-C86A-40BC-81CB-2B4FC4C86603}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
@@ -38448,7 +38451,7 @@
       <c r="D1" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="91" t="s">
+      <c r="E1" s="125" t="s">
         <v>53</v>
       </c>
       <c r="F1" s="91" t="s">
@@ -38468,10 +38471,11 @@
       <c r="D2" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="91">
+      <c r="E2" s="125">
         <v>4</v>
       </c>
       <c r="F2" s="91">
+        <f>IF(E2=4,1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -38488,10 +38492,11 @@
       <c r="D3" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="91">
+      <c r="E3" s="125">
         <v>4</v>
       </c>
       <c r="F3" s="91">
+        <f t="shared" ref="F3:F42" si="0">IF(E3=4,1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -38508,10 +38513,11 @@
       <c r="D4" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="91">
+      <c r="E4" s="125">
         <v>4</v>
       </c>
       <c r="F4" s="91">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -38528,10 +38534,11 @@
       <c r="D5" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="91">
+      <c r="E5" s="125">
         <v>4</v>
       </c>
       <c r="F5" s="91">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -38548,11 +38555,12 @@
       <c r="D6" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="91">
-        <v>4</v>
+      <c r="E6" s="125">
+        <v>3</v>
       </c>
       <c r="F6" s="91">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -38568,10 +38576,11 @@
       <c r="D7" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="91">
+      <c r="E7" s="125">
         <v>4</v>
       </c>
       <c r="F7" s="91">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -38588,10 +38597,11 @@
       <c r="D8" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="91">
+      <c r="E8" s="125">
         <v>4</v>
       </c>
       <c r="F8" s="91">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -38608,11 +38618,12 @@
       <c r="D9" s="91" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="91">
-        <v>2</v>
+      <c r="E9" s="125">
+        <v>4</v>
       </c>
       <c r="F9" s="91">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -38628,10 +38639,11 @@
       <c r="D10" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="91">
+      <c r="E10" s="125">
         <v>4</v>
       </c>
       <c r="F10" s="91">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -38648,10 +38660,11 @@
       <c r="D11" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="91">
+      <c r="E11" s="125">
         <v>4</v>
       </c>
       <c r="F11" s="91">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -38668,10 +38681,11 @@
       <c r="D12" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="91">
+      <c r="E12" s="125">
         <v>4</v>
       </c>
       <c r="F12" s="91">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -38688,10 +38702,11 @@
       <c r="D13" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="E13" s="91">
+      <c r="E13" s="125">
         <v>4</v>
       </c>
       <c r="F13" s="91">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -38708,10 +38723,11 @@
       <c r="D14" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="91">
+      <c r="E14" s="125">
         <v>4</v>
       </c>
       <c r="F14" s="91">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -38728,10 +38744,11 @@
       <c r="D15" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="91">
+      <c r="E15" s="125">
         <v>4</v>
       </c>
       <c r="F15" s="91">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -38748,10 +38765,11 @@
       <c r="D16" s="91" t="s">
         <v>63</v>
       </c>
-      <c r="E16" s="91">
+      <c r="E16" s="125">
         <v>4</v>
       </c>
       <c r="F16" s="91">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -38768,10 +38786,11 @@
       <c r="D17" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="E17" s="91">
+      <c r="E17" s="125">
         <v>4</v>
       </c>
       <c r="F17" s="91">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -38788,10 +38807,11 @@
       <c r="D18" s="91" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="91">
+      <c r="E18" s="125">
         <v>4</v>
       </c>
       <c r="F18" s="91">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -38808,10 +38828,11 @@
       <c r="D19" s="91" t="s">
         <v>65</v>
       </c>
-      <c r="E19" s="91">
+      <c r="E19" s="125">
         <v>4</v>
       </c>
       <c r="F19" s="91">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -38828,10 +38849,11 @@
       <c r="D20" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="E20" s="91">
+      <c r="E20" s="125">
         <v>4</v>
       </c>
       <c r="F20" s="91">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -38848,10 +38870,11 @@
       <c r="D21" s="91" t="s">
         <v>63</v>
       </c>
-      <c r="E21" s="91">
+      <c r="E21" s="125">
         <v>4</v>
       </c>
       <c r="F21" s="91">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -38868,10 +38891,11 @@
       <c r="D22" s="91" t="s">
         <v>63</v>
       </c>
-      <c r="E22" s="91">
+      <c r="E22" s="125">
         <v>4</v>
       </c>
       <c r="F22" s="91">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -38888,10 +38912,11 @@
       <c r="D23" s="91" t="s">
         <v>63</v>
       </c>
-      <c r="E23" s="91">
+      <c r="E23" s="125">
         <v>4</v>
       </c>
       <c r="F23" s="91">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -38908,10 +38933,11 @@
       <c r="D24" s="91" t="s">
         <v>63</v>
       </c>
-      <c r="E24" s="91">
+      <c r="E24" s="125">
         <v>4</v>
       </c>
       <c r="F24" s="91">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -38928,10 +38954,11 @@
       <c r="D25" s="91" t="s">
         <v>63</v>
       </c>
-      <c r="E25" s="91">
+      <c r="E25" s="125">
         <v>4</v>
       </c>
       <c r="F25" s="91">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -38948,10 +38975,11 @@
       <c r="D26" s="91" t="s">
         <v>65</v>
       </c>
-      <c r="E26" s="91">
+      <c r="E26" s="125">
         <v>4</v>
       </c>
       <c r="F26" s="91">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -38968,10 +38996,11 @@
       <c r="D27" s="91" t="s">
         <v>63</v>
       </c>
-      <c r="E27" s="91">
+      <c r="E27" s="125">
         <v>4</v>
       </c>
       <c r="F27" s="91">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -38988,11 +39017,12 @@
       <c r="D28" s="91" t="s">
         <v>65</v>
       </c>
-      <c r="E28" s="91">
-        <v>4</v>
+      <c r="E28" s="125">
+        <v>3</v>
       </c>
       <c r="F28" s="91">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -39008,10 +39038,11 @@
       <c r="D29" s="91" t="s">
         <v>65</v>
       </c>
-      <c r="E29" s="91">
+      <c r="E29" s="125">
         <v>2</v>
       </c>
       <c r="F29" s="91">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -39028,10 +39059,11 @@
       <c r="D30" s="91" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="91">
+      <c r="E30" s="125">
         <v>2</v>
       </c>
       <c r="F30" s="91">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -39048,10 +39080,11 @@
       <c r="D31" s="91" t="s">
         <v>63</v>
       </c>
-      <c r="E31" s="91">
+      <c r="E31" s="125">
         <v>2</v>
       </c>
       <c r="F31" s="91">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -39068,10 +39101,11 @@
       <c r="D32" s="91" t="s">
         <v>65</v>
       </c>
-      <c r="E32" s="91">
+      <c r="E32" s="125">
         <v>2</v>
       </c>
       <c r="F32" s="91">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -39088,11 +39122,12 @@
       <c r="D33" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="E33" s="91">
-        <v>2</v>
+      <c r="E33" s="125">
+        <v>4</v>
       </c>
       <c r="F33" s="91">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -39108,10 +39143,11 @@
       <c r="D34" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="E34" s="91">
+      <c r="E34" s="125">
         <v>4</v>
       </c>
       <c r="F34" s="91">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -39128,10 +39164,11 @@
       <c r="D35" s="91" t="s">
         <v>63</v>
       </c>
-      <c r="E35" s="91">
+      <c r="E35" s="125">
         <v>4</v>
       </c>
       <c r="F35" s="91">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -39148,10 +39185,11 @@
       <c r="D36" s="91" t="s">
         <v>63</v>
       </c>
-      <c r="E36" s="91">
+      <c r="E36" s="125">
         <v>4</v>
       </c>
       <c r="F36" s="91">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -39168,10 +39206,11 @@
       <c r="D37" s="91" t="s">
         <v>63</v>
       </c>
-      <c r="E37" s="91">
+      <c r="E37" s="125">
         <v>4</v>
       </c>
       <c r="F37" s="91">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -39188,10 +39227,11 @@
       <c r="D38" s="91" t="s">
         <v>65</v>
       </c>
-      <c r="E38" s="91">
+      <c r="E38" s="125">
         <v>4</v>
       </c>
       <c r="F38" s="91">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -39208,10 +39248,11 @@
       <c r="D39" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="E39" s="91">
+      <c r="E39" s="125">
         <v>4</v>
       </c>
       <c r="F39" s="91">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -39228,10 +39269,11 @@
       <c r="D40" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="E40" s="91">
+      <c r="E40" s="125">
         <v>4</v>
       </c>
       <c r="F40" s="91">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -39248,10 +39290,11 @@
       <c r="D41" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="E41" s="91">
+      <c r="E41" s="125">
         <v>4</v>
       </c>
       <c r="F41" s="91">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -39268,10 +39311,11 @@
       <c r="D42" s="91" t="s">
         <v>63</v>
       </c>
-      <c r="E42" s="91">
+      <c r="E42" s="125">
         <v>4</v>
       </c>
       <c r="F42" s="91">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -69729,6 +69773,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010008F661E3DE9C25499C21C40FDF902C8B" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1b68ea25bc605e38c2d03e877024c293">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ee290c57-2ef8-46a0-8529-ed69fb4a5f2c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3cf02698435ed336187c95b5e1c58beb" ns2:_="">
     <xsd:import namespace="ee290c57-2ef8-46a0-8529-ed69fb4a5f2c"/>
@@ -69868,12 +69918,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CF4104A-3DED-4E2C-8A09-5465BE014F85}">
   <ds:schemaRefs>
@@ -69883,6 +69927,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAF3E1FB-3FB7-45B8-895A-91622E2DB3CE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ee290c57-2ef8-46a0-8529-ed69fb4a5f2c"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3320A65C-F914-4909-98B2-D44984893BBC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -69898,20 +69958,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAF3E1FB-3FB7-45B8-895A-91622E2DB3CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ee290c57-2ef8-46a0-8529-ed69fb4a5f2c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>